<commit_message>
(#157) Added print page tests
</commit_message>
<xml_diff>
--- a/test-data/cts-search-results-data.xlsx
+++ b/test-data/cts-search-results-data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashkinaea/IdeaProjects/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276FE539-686A-584B-9F55-C74A4A395CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5012E117-CEFF-8442-A6DE-9808920E0429}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" xr2:uid="{29D48476-2BE1-4547-8429-BC5CC2E327E5}"/>
+    <workbookView xWindow="31800" yWindow="5160" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{29D48476-2BE1-4547-8429-BC5CC2E327E5}"/>
   </bookViews>
   <sheets>
     <sheet name="search_results_pages" sheetId="1" r:id="rId1"/>
     <sheet name="search_results_negative" sheetId="2" r:id="rId2"/>
+    <sheet name="print_page" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="60">
   <si>
     <t>path</t>
   </si>
@@ -198,6 +199,27 @@
   </si>
   <si>
     <t>Status:Active</t>
+  </si>
+  <si>
+    <t>about-cancer/treatment/clinical-trials/search/r?loc=0&amp;rl=1</t>
+  </si>
+  <si>
+    <t>printLink</t>
+  </si>
+  <si>
+    <t>emailLink</t>
+  </si>
+  <si>
+    <t>newSearchLink</t>
+  </si>
+  <si>
+    <t>/common/popUps/PopEmail.aspx</t>
+  </si>
+  <si>
+    <t>javascript:window.print();</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/clinical-trials/advanced-search</t>
   </si>
 </sst>
 </file>
@@ -576,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482B77C0-B496-EE4B-98D3-F6A3D360AB8F}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F2E912-05AB-044E-B414-E9AE6E18C18C}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1054,4 +1076,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023F48AD-DC30-3641-96FD-89D60DF300B0}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>